<commit_message>
flickernoise tolerances compact qual
</commit_message>
<xml_diff>
--- a/compact_measurement/library_qualification_tolerances.xlsx
+++ b/compact_measurement/library_qualification_tolerances.xlsx
@@ -599,10 +599,10 @@
   <dimension ref="A1:Q55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L26" sqref="L26"/>
+      <selection pane="bottomRight" activeCell="M52" sqref="M52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.2"/>
@@ -1851,7 +1851,7 @@
         <v>2E-3</v>
       </c>
       <c r="O48" s="3">
-        <v>0.02</v>
+        <v>3.9999999999999998E-7</v>
       </c>
     </row>
     <row r="49" spans="1:15">

</xml_diff>